<commit_message>
Excel read function added
</commit_message>
<xml_diff>
--- a/CW_Automation/CW_Automation/TestData/CW_Data_Sheet.xlsx
+++ b/CW_Automation/CW_Automation/TestData/CW_Data_Sheet.xlsx
@@ -21,135 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
-    <t>Sr. No.</t>
-  </si>
-  <si>
-    <t>Test Case Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Parameter 1</t>
-  </si>
-  <si>
-    <t>Value 1</t>
-  </si>
-  <si>
-    <t>Parameter 2</t>
-  </si>
-  <si>
-    <t>Value 2</t>
-  </si>
-  <si>
-    <t>Parameter 3</t>
-  </si>
-  <si>
-    <t>Value 3</t>
-  </si>
-  <si>
-    <t>Parameter 4</t>
-  </si>
-  <si>
-    <t>Value 4</t>
-  </si>
-  <si>
-    <t>Parameter 5</t>
-  </si>
-  <si>
-    <t>Value 5</t>
-  </si>
-  <si>
-    <t>Parameter 6</t>
-  </si>
-  <si>
-    <t>Value 6</t>
-  </si>
-  <si>
-    <t>Parameter 7</t>
-  </si>
-  <si>
-    <t>Value 7</t>
-  </si>
-  <si>
-    <t>Parameter 8</t>
-  </si>
-  <si>
-    <t>Value 8</t>
-  </si>
-  <si>
-    <t>Parameter 9</t>
-  </si>
-  <si>
-    <t>Value 9</t>
-  </si>
-  <si>
-    <t>Parameter 10</t>
-  </si>
-  <si>
-    <t>Value 10</t>
-  </si>
-  <si>
-    <t>Parameter 11</t>
-  </si>
-  <si>
-    <t>Value 11</t>
-  </si>
-  <si>
-    <t>Parameter 12</t>
-  </si>
-  <si>
-    <t>Value 12</t>
-  </si>
-  <si>
-    <t>Parameter 13</t>
-  </si>
-  <si>
-    <t>Value 13</t>
-  </si>
-  <si>
-    <t>Parameter 14</t>
-  </si>
-  <si>
-    <t>Value 14</t>
-  </si>
-  <si>
-    <t>Parameter 15</t>
-  </si>
-  <si>
-    <t>Value 15</t>
-  </si>
-  <si>
-    <t>Parameter 16</t>
-  </si>
-  <si>
-    <t>Value 16</t>
-  </si>
-  <si>
-    <t>Parameter 17</t>
-  </si>
-  <si>
-    <t>Value 17</t>
-  </si>
-  <si>
-    <t>Parameter 18</t>
-  </si>
-  <si>
-    <t>Value 18</t>
-  </si>
-  <si>
-    <t>Parameter 19</t>
-  </si>
-  <si>
-    <t>Value 19</t>
-  </si>
-  <si>
-    <t>Parameter 20</t>
-  </si>
-  <si>
-    <t>Value 20</t>
-  </si>
-  <si>
     <t>Create Slings Web equipment</t>
   </si>
   <si>
@@ -172,6 +43,135 @@
   </si>
   <si>
     <t>001</t>
+  </si>
+  <si>
+    <t>SR. NO.</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Parameter1</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Parameter2</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Parameter3</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>Parameter4</t>
+  </si>
+  <si>
+    <t>Value4</t>
+  </si>
+  <si>
+    <t>Parameter5</t>
+  </si>
+  <si>
+    <t>Value5</t>
+  </si>
+  <si>
+    <t>Parameter6</t>
+  </si>
+  <si>
+    <t>Value6</t>
+  </si>
+  <si>
+    <t>Parameter7</t>
+  </si>
+  <si>
+    <t>Value7</t>
+  </si>
+  <si>
+    <t>Parameter8</t>
+  </si>
+  <si>
+    <t>Value8</t>
+  </si>
+  <si>
+    <t>Parameter9</t>
+  </si>
+  <si>
+    <t>Value9</t>
+  </si>
+  <si>
+    <t>Parameter10</t>
+  </si>
+  <si>
+    <t>Value10</t>
+  </si>
+  <si>
+    <t>Parameter11</t>
+  </si>
+  <si>
+    <t>Value11</t>
+  </si>
+  <si>
+    <t>Parameter12</t>
+  </si>
+  <si>
+    <t>Value12</t>
+  </si>
+  <si>
+    <t>Parameter13</t>
+  </si>
+  <si>
+    <t>Value13</t>
+  </si>
+  <si>
+    <t>Parameter14</t>
+  </si>
+  <si>
+    <t>Value14</t>
+  </si>
+  <si>
+    <t>Parameter15</t>
+  </si>
+  <si>
+    <t>Value15</t>
+  </si>
+  <si>
+    <t>Parameter16</t>
+  </si>
+  <si>
+    <t>Value16</t>
+  </si>
+  <si>
+    <t>Parameter17</t>
+  </si>
+  <si>
+    <t>Value17</t>
+  </si>
+  <si>
+    <t>Parameter18</t>
+  </si>
+  <si>
+    <t>Value18</t>
+  </si>
+  <si>
+    <t>Parameter19</t>
+  </si>
+  <si>
+    <t>Value19</t>
+  </si>
+  <si>
+    <t>Parameter20</t>
+  </si>
+  <si>
+    <t>Value20</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,174 +502,199 @@
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="W1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="X1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="Z1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="AA1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="AB1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="AC1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="AD1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="AE1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="AF1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="AG1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="AH1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AI1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="AJ1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="AK1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="AL1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="AM1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AN1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="AO1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AP1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AQ1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>123456789</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="K2" s="2">
         <f ca="1">TODAY()</f>
-        <v>43622</v>
+        <v>43627</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>